<commit_message>
ADD: CONNECT XLSX FIX: DSM and NETWORK
</commit_message>
<xml_diff>
--- a/excel/General_Label_Matrix.xlsx
+++ b/excel/General_Label_Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hideakiozawa/Desktop/Generating_Specification_Standard/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CAEEDE-CA31-1B44-8C9A-5E04969E46DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B248EF53-C4E0-9148-915E-CFECD75BC074}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="1460" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="820" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="label_list" sheetId="1" r:id="rId1"/>
@@ -782,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA99"/>
+  <dimension ref="A1:AA100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -9007,6 +9007,86 @@
         <v>29</v>
       </c>
     </row>
+    <row r="100" spans="1:27">
+      <c r="B100">
+        <v>4</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100">
+        <v>8</v>
+      </c>
+      <c r="E100">
+        <v>10</v>
+      </c>
+      <c r="F100">
+        <v>5</v>
+      </c>
+      <c r="G100">
+        <v>2</v>
+      </c>
+      <c r="H100">
+        <v>3</v>
+      </c>
+      <c r="I100">
+        <v>3</v>
+      </c>
+      <c r="J100">
+        <v>4</v>
+      </c>
+      <c r="K100">
+        <v>5</v>
+      </c>
+      <c r="L100">
+        <v>4</v>
+      </c>
+      <c r="M100">
+        <v>3</v>
+      </c>
+      <c r="N100">
+        <v>2</v>
+      </c>
+      <c r="O100">
+        <v>5</v>
+      </c>
+      <c r="P100">
+        <v>2</v>
+      </c>
+      <c r="Q100">
+        <v>4</v>
+      </c>
+      <c r="R100">
+        <v>3</v>
+      </c>
+      <c r="S100">
+        <v>3</v>
+      </c>
+      <c r="T100">
+        <v>4</v>
+      </c>
+      <c r="U100">
+        <v>1</v>
+      </c>
+      <c r="V100">
+        <v>1</v>
+      </c>
+      <c r="W100">
+        <v>6</v>
+      </c>
+      <c r="X100">
+        <v>2</v>
+      </c>
+      <c r="Y100">
+        <v>4</v>
+      </c>
+      <c r="Z100">
+        <v>3</v>
+      </c>
+      <c r="AA100">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AA99" xr:uid="{507ECBA1-269E-8A4B-96A3-746DF97D9929}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA99">

</xml_diff>